<commit_message>
Creazione Gantt e inizio sviluppo interfaccia
</commit_message>
<xml_diff>
--- a/Allegati/Requisiti.xlsx
+++ b/Allegati/Requisiti.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paolo\workspace\CPTRoverControl\Allegati\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26AEBC5-D658-42B3-ACA9-56734CAC649A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFF7383-2615-4D40-A8D0-F1DF694B1136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>Descrizione del requisito</t>
   </si>
@@ -40,14 +40,6 @@
   </si>
   <si>
     <t>Priorità di implementazione</t>
-  </si>
-  <si>
-    <t>Importanza del requisito nell'ambito dello specifico progetto, dal punto di vista del richiedente. Valori esemplificativi:
-1 – essenziale
-2 - molto importante
-3 - importante
-4 - abbastanza importante
-5 - secondario</t>
   </si>
   <si>
     <t>Priorità temporale attribuita dal richiedente per l'implementazione del requisito, utilizzabile dai progettisti in un'ottica di rilasci incrementali. Valori esemplificativi:
@@ -253,9 +245,6 @@
     </r>
   </si>
   <si>
-    <t>2 dettaglia 1</t>
-  </si>
-  <si>
     <t>Forgia Paolo</t>
   </si>
   <si>
@@ -268,28 +257,65 @@
 - eliminato</t>
   </si>
   <si>
-    <t>L'applicativo deve girare su smartphone e tablet</t>
-  </si>
-  <si>
-    <t>Bisogna sviluppare un solo applicativo che gira su tutte le piattaforme</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>L'app deve connettersi via bluetooth al rover</t>
-  </si>
-  <si>
     <t>L'app deve trasmettere comandi al rover</t>
   </si>
   <si>
     <t>L'app deve ricevere comandi dal rover</t>
   </si>
   <si>
-    <t>4 dipende da 3</t>
-  </si>
-  <si>
-    <t>5 dipende da 3</t>
+    <t>L'applicativo deve girare su smartphone</t>
+  </si>
+  <si>
+    <t>L'applicativo deve girare su tablet</t>
+  </si>
+  <si>
+    <t>L'app deve connettersi via Bluetooth al rover</t>
+  </si>
+  <si>
+    <t>L'applicativo deve funzionare su Android e iOS</t>
+  </si>
+  <si>
+    <t>eliminato</t>
+  </si>
+  <si>
+    <t>L'applicativo deve funzionare solo su Android</t>
+  </si>
+  <si>
+    <t>3 dettaglia 1</t>
+  </si>
+  <si>
+    <t>5 dipende da 4</t>
+  </si>
+  <si>
+    <t>6 dipende da 4</t>
+  </si>
+  <si>
+    <t>9 sostituisce 3</t>
+  </si>
+  <si>
+    <t>concordato</t>
+  </si>
+  <si>
+    <t>L'interfaccia deve mostrare le informazioni ritornate dal rover</t>
+  </si>
+  <si>
+    <t>L'interfaccia deve poter controllare il rover in tutte le sue funzionalità</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Importanza del requisito nell'ambito dello specifico progetto, dal punto di vista del richiedente. Valori esemplificativi:
+1 – essenziale
+2 - molto importante
+3 - importante
+4 - secondario</t>
   </si>
 </sst>
 </file>
@@ -452,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -595,9 +621,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -993,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV12"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1005,33 +1028,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="64"/>
+      <c r="A1" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="63"/>
     </row>
     <row r="2" spans="1:256" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:256" s="37" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:256" s="8" customFormat="1" ht="333.75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -1304,12 +1327,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:256" s="1" customFormat="1" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:256" s="1" customFormat="1" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:256" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
@@ -1317,23 +1340,23 @@
         <v>4</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:256" ht="57" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>7</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:256" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:256" x14ac:dyDescent="0.2">
@@ -1358,17 +1381,17 @@
   <dimension ref="A1:BA39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E1" sqref="E1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.28515625" style="31" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" style="31" customWidth="1"/>
-    <col min="3" max="3" width="76.7109375" style="63" customWidth="1"/>
+    <col min="3" max="3" width="76.7109375" style="62" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" style="48" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" style="48" customWidth="1"/>
-    <col min="6" max="6" width="19" style="50" customWidth="1"/>
+    <col min="6" max="6" width="19" style="49" customWidth="1"/>
     <col min="7" max="7" width="17" style="43" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" style="43" bestFit="1" customWidth="1"/>
     <col min="9" max="52" width="8.85546875" style="23"/>
@@ -1377,22 +1400,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="56" t="s">
-        <v>18</v>
+      <c r="A1" s="55" t="s">
+        <v>17</v>
       </c>
       <c r="B1" s="32"/>
-      <c r="C1" s="57" t="s">
-        <v>21</v>
+      <c r="C1" s="56" t="s">
+        <v>19</v>
       </c>
       <c r="D1" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="65">
-        <v>44743</v>
-      </c>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="67"/>
+        <v>13</v>
+      </c>
+      <c r="E1" s="64">
+        <v>44806</v>
+      </c>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="66"/>
       <c r="I1" s="20"/>
       <c r="J1" s="20"/>
       <c r="K1" s="20"/>
@@ -1442,7 +1465,7 @@
     <row r="2" spans="1:53" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="33"/>
       <c r="B2" s="33"/>
-      <c r="C2" s="58"/>
+      <c r="C2" s="57"/>
       <c r="D2" s="44"/>
       <c r="E2" s="44"/>
       <c r="F2" s="44"/>
@@ -1494,96 +1517,100 @@
       <c r="AZ2" s="21"/>
       <c r="BA2" s="26"/>
     </row>
-    <row r="3" spans="1:53" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:53" s="54" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="51" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="D3" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="E3" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="51" t="s">
+      <c r="F3" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="51" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="53"/>
-      <c r="S3" s="53"/>
-      <c r="T3" s="53"/>
-      <c r="U3" s="53"/>
-      <c r="V3" s="53"/>
-      <c r="W3" s="53"/>
-      <c r="X3" s="53"/>
-      <c r="Y3" s="53"/>
-      <c r="Z3" s="53"/>
-      <c r="AA3" s="53"/>
-      <c r="AB3" s="53"/>
-      <c r="AC3" s="53"/>
-      <c r="AD3" s="53"/>
-      <c r="AE3" s="53"/>
-      <c r="AF3" s="53"/>
-      <c r="AG3" s="53"/>
-      <c r="AH3" s="53"/>
-      <c r="AI3" s="53"/>
-      <c r="AJ3" s="53"/>
-      <c r="AK3" s="53"/>
-      <c r="AL3" s="53"/>
-      <c r="AM3" s="53"/>
-      <c r="AN3" s="53"/>
-      <c r="AO3" s="53"/>
-      <c r="AP3" s="53"/>
-      <c r="AQ3" s="53"/>
-      <c r="AR3" s="53"/>
-      <c r="AS3" s="53"/>
-      <c r="AT3" s="53"/>
-      <c r="AU3" s="53"/>
-      <c r="AV3" s="53"/>
-      <c r="AW3" s="53"/>
-      <c r="AX3" s="53"/>
-      <c r="AY3" s="53"/>
-      <c r="AZ3" s="53"/>
-      <c r="BA3" s="54"/>
+      <c r="G3" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="52"/>
+      <c r="Q3" s="52"/>
+      <c r="R3" s="52"/>
+      <c r="S3" s="52"/>
+      <c r="T3" s="52"/>
+      <c r="U3" s="52"/>
+      <c r="V3" s="52"/>
+      <c r="W3" s="52"/>
+      <c r="X3" s="52"/>
+      <c r="Y3" s="52"/>
+      <c r="Z3" s="52"/>
+      <c r="AA3" s="52"/>
+      <c r="AB3" s="52"/>
+      <c r="AC3" s="52"/>
+      <c r="AD3" s="52"/>
+      <c r="AE3" s="52"/>
+      <c r="AF3" s="52"/>
+      <c r="AG3" s="52"/>
+      <c r="AH3" s="52"/>
+      <c r="AI3" s="52"/>
+      <c r="AJ3" s="52"/>
+      <c r="AK3" s="52"/>
+      <c r="AL3" s="52"/>
+      <c r="AM3" s="52"/>
+      <c r="AN3" s="52"/>
+      <c r="AO3" s="52"/>
+      <c r="AP3" s="52"/>
+      <c r="AQ3" s="52"/>
+      <c r="AR3" s="52"/>
+      <c r="AS3" s="52"/>
+      <c r="AT3" s="52"/>
+      <c r="AU3" s="52"/>
+      <c r="AV3" s="52"/>
+      <c r="AW3" s="52"/>
+      <c r="AX3" s="52"/>
+      <c r="AY3" s="52"/>
+      <c r="AZ3" s="52"/>
+      <c r="BA3" s="53"/>
     </row>
     <row r="4" spans="1:53" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="30">
         <v>1</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="59" t="s">
+      <c r="B4" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="52">
-        <v>44743</v>
-      </c>
-      <c r="E4" s="46">
+      <c r="D4" s="51">
+        <v>44806</v>
+      </c>
+      <c r="E4" s="47">
         <v>1</v>
       </c>
       <c r="F4" s="46">
         <v>1</v>
       </c>
       <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
+      <c r="H4" s="40" t="s">
+        <v>33</v>
+      </c>
       <c r="I4" s="19"/>
       <c r="J4" s="19"/>
       <c r="K4" s="19"/>
@@ -1635,24 +1662,23 @@
         <v>2</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="60" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="52">
-        <v>44743</v>
+      <c r="D5" s="51">
+        <v>44806</v>
       </c>
       <c r="E5" s="47">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F5" s="47">
-        <v>1</v>
-      </c>
-      <c r="G5" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="40"/>
+        <v>3</v>
+      </c>
+      <c r="H5" s="40" t="s">
+        <v>33</v>
+      </c>
       <c r="I5" s="19"/>
       <c r="J5" s="19"/>
       <c r="K5" s="19"/>
@@ -1703,12 +1729,14 @@
       <c r="A6" s="30">
         <v>3</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="61" t="s">
+      <c r="B6" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="52">
-        <v>44743</v>
+      <c r="D6" s="51">
+        <v>44806</v>
       </c>
       <c r="E6" s="47">
         <v>1</v>
@@ -1716,8 +1744,12 @@
       <c r="F6" s="47">
         <v>1</v>
       </c>
-      <c r="G6" s="41"/>
-      <c r="H6" s="40"/>
+      <c r="G6" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="40" t="s">
+        <v>27</v>
+      </c>
       <c r="I6" s="19"/>
       <c r="J6" s="19"/>
       <c r="K6" s="19"/>
@@ -1768,12 +1800,14 @@
       <c r="A7" s="30">
         <v>4</v>
       </c>
-      <c r="B7" s="30"/>
+      <c r="B7" s="30" t="s">
+        <v>37</v>
+      </c>
       <c r="C7" s="60" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="52">
-        <v>44743</v>
+        <v>25</v>
+      </c>
+      <c r="D7" s="51">
+        <v>44806</v>
       </c>
       <c r="E7" s="47">
         <v>1</v>
@@ -1781,10 +1815,10 @@
       <c r="F7" s="47">
         <v>2</v>
       </c>
-      <c r="G7" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="40"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="40" t="s">
+        <v>33</v>
+      </c>
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
       <c r="K7" s="19"/>
@@ -1835,15 +1869,17 @@
       <c r="A8" s="30">
         <v>5</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="52">
-        <v>44743</v>
+      <c r="B8" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="59" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="51">
+        <v>44806</v>
       </c>
       <c r="E8" s="47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" s="47">
         <v>2</v>
@@ -1851,7 +1887,9 @@
       <c r="G8" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="40"/>
+      <c r="H8" s="40" t="s">
+        <v>33</v>
+      </c>
       <c r="I8" s="19"/>
       <c r="J8" s="19"/>
       <c r="K8" s="19"/>
@@ -1902,13 +1940,27 @@
       <c r="A9" s="30">
         <v>6</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="40"/>
+      <c r="B9" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="51">
+        <v>44806</v>
+      </c>
+      <c r="E9" s="47">
+        <v>2</v>
+      </c>
+      <c r="F9" s="47">
+        <v>3</v>
+      </c>
+      <c r="G9" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="40" t="s">
+        <v>33</v>
+      </c>
       <c r="I9" s="19"/>
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
@@ -1959,13 +2011,24 @@
       <c r="A10" s="30">
         <v>7</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="40"/>
+      <c r="B10" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="51">
+        <v>44806</v>
+      </c>
+      <c r="E10" s="47">
+        <v>3</v>
+      </c>
+      <c r="F10" s="47">
+        <v>3</v>
+      </c>
+      <c r="H10" s="40" t="s">
+        <v>33</v>
+      </c>
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
@@ -2016,13 +2079,25 @@
       <c r="A11" s="30">
         <v>8</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
+      <c r="B11" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="51">
+        <v>44806</v>
+      </c>
+      <c r="E11" s="47">
+        <v>2</v>
+      </c>
+      <c r="F11" s="47">
+        <v>2</v>
+      </c>
       <c r="G11" s="41"/>
-      <c r="H11" s="40"/>
+      <c r="H11" s="40" t="s">
+        <v>33</v>
+      </c>
       <c r="I11" s="19"/>
       <c r="J11" s="19"/>
       <c r="K11" s="19"/>
@@ -2073,13 +2148,27 @@
       <c r="A12" s="30">
         <v>9</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="40"/>
+      <c r="B12" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="51">
+        <v>44813</v>
+      </c>
+      <c r="E12" s="47">
+        <v>1</v>
+      </c>
+      <c r="F12" s="47">
+        <v>1</v>
+      </c>
+      <c r="G12" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="40" t="s">
+        <v>33</v>
+      </c>
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
@@ -2131,8 +2220,8 @@
         <v>10</v>
       </c>
       <c r="B13" s="30"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="52"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="51"/>
       <c r="E13" s="47"/>
       <c r="F13" s="47"/>
       <c r="G13" s="41"/>
@@ -2188,8 +2277,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="30"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="52"/>
+      <c r="D14" s="51"/>
       <c r="E14" s="47"/>
       <c r="F14" s="47"/>
       <c r="G14" s="41"/>
@@ -2245,8 +2333,8 @@
         <v>12</v>
       </c>
       <c r="B15" s="30"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="52"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="51"/>
       <c r="E15" s="47"/>
       <c r="F15" s="47"/>
       <c r="G15" s="41"/>
@@ -2302,8 +2390,8 @@
         <v>13</v>
       </c>
       <c r="B16" s="30"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="52"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="51"/>
       <c r="E16" s="47"/>
       <c r="F16" s="47"/>
       <c r="G16" s="41"/>
@@ -2359,8 +2447,8 @@
         <v>14</v>
       </c>
       <c r="B17" s="30"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="52"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="51"/>
       <c r="E17" s="47"/>
       <c r="F17" s="47"/>
       <c r="G17" s="41"/>
@@ -2416,8 +2504,8 @@
         <v>15</v>
       </c>
       <c r="B18" s="30"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="52"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="51"/>
       <c r="E18" s="47"/>
       <c r="F18" s="47"/>
       <c r="G18" s="41"/>
@@ -2473,8 +2561,8 @@
         <v>16</v>
       </c>
       <c r="B19" s="30"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="52"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="51"/>
       <c r="E19" s="47"/>
       <c r="F19" s="47"/>
       <c r="G19" s="41"/>
@@ -2530,7 +2618,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="30"/>
-      <c r="C20" s="61"/>
+      <c r="C20" s="60"/>
       <c r="D20" s="47"/>
       <c r="E20" s="47"/>
       <c r="F20" s="47"/>
@@ -2587,7 +2675,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="30"/>
-      <c r="C21" s="60"/>
+      <c r="C21" s="59"/>
       <c r="D21" s="47"/>
       <c r="E21" s="47"/>
       <c r="F21" s="47"/>
@@ -2644,7 +2732,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="30"/>
-      <c r="C22" s="61"/>
+      <c r="C22" s="60"/>
       <c r="D22" s="47"/>
       <c r="E22" s="47"/>
       <c r="F22" s="47"/>
@@ -2699,7 +2787,7 @@
     <row r="23" spans="1:53" s="16" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="30"/>
       <c r="B23" s="30"/>
-      <c r="C23" s="61"/>
+      <c r="C23" s="60"/>
       <c r="D23" s="47"/>
       <c r="E23" s="47"/>
       <c r="F23" s="47"/>
@@ -2754,7 +2842,7 @@
     <row r="24" spans="1:53" s="16" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A24" s="30"/>
       <c r="B24" s="30"/>
-      <c r="C24" s="61"/>
+      <c r="C24" s="60"/>
       <c r="D24" s="47"/>
       <c r="E24" s="47"/>
       <c r="F24" s="47"/>
@@ -2809,7 +2897,7 @@
     <row r="25" spans="1:53" s="16" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A25" s="30"/>
       <c r="B25" s="30"/>
-      <c r="C25" s="61"/>
+      <c r="C25" s="60"/>
       <c r="D25" s="47"/>
       <c r="E25" s="47"/>
       <c r="F25" s="47"/>
@@ -2864,7 +2952,7 @@
     <row r="26" spans="1:53" s="16" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A26" s="30"/>
       <c r="B26" s="30"/>
-      <c r="C26" s="61"/>
+      <c r="C26" s="60"/>
       <c r="D26" s="47"/>
       <c r="E26" s="47"/>
       <c r="F26" s="47"/>
@@ -2919,7 +3007,7 @@
     <row r="27" spans="1:53" s="16" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A27" s="30"/>
       <c r="B27" s="30"/>
-      <c r="C27" s="61"/>
+      <c r="C27" s="60"/>
       <c r="D27" s="47"/>
       <c r="E27" s="47"/>
       <c r="F27" s="47"/>
@@ -2974,7 +3062,7 @@
     <row r="28" spans="1:53" s="16" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A28" s="30"/>
       <c r="B28" s="30"/>
-      <c r="C28" s="60"/>
+      <c r="C28" s="59"/>
       <c r="D28" s="47"/>
       <c r="E28" s="47"/>
       <c r="F28" s="47"/>
@@ -3029,10 +3117,10 @@
     <row r="29" spans="1:53" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A29" s="30"/>
       <c r="B29" s="30"/>
-      <c r="C29" s="62"/>
+      <c r="C29" s="61"/>
       <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="49"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
       <c r="G29" s="42"/>
       <c r="H29" s="42"/>
       <c r="I29" s="22"/>
@@ -3084,10 +3172,10 @@
     <row r="30" spans="1:53" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A30" s="30"/>
       <c r="B30" s="30"/>
-      <c r="C30" s="62"/>
+      <c r="C30" s="61"/>
       <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="49"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
       <c r="G30" s="42"/>
       <c r="H30" s="42"/>
       <c r="I30" s="22"/>
@@ -3139,10 +3227,10 @@
     <row r="31" spans="1:53" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A31" s="30"/>
       <c r="B31" s="30"/>
-      <c r="C31" s="62"/>
+      <c r="C31" s="61"/>
       <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="49"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
       <c r="G31" s="42"/>
       <c r="H31" s="42"/>
       <c r="I31" s="22"/>
@@ -3194,41 +3282,63 @@
     <row r="32" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A32" s="34"/>
       <c r="B32" s="34"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="34"/>
       <c r="B33" s="34"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E33" s="47"/>
+      <c r="F33" s="47"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="34"/>
       <c r="B34" s="34"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E34" s="47"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="34"/>
       <c r="B35" s="34"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E35" s="46"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="34"/>
       <c r="B36" s="34"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E36" s="46"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="34"/>
       <c r="B37" s="34"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E37" s="46"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="34"/>
       <c r="B38" s="34"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E38" s="46"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="34"/>
       <c r="B39" s="34"/>
+      <c r="E39" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E1:H1"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="E4">
+  <conditionalFormatting sqref="E25:E39">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E3 E25:E65536">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -3240,8 +3350,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E65536">
-    <cfRule type="colorScale" priority="5">
+  <conditionalFormatting sqref="F2:F65536">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3252,8 +3362,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F65536">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="E4:E34">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
Added test (not yet working)
</commit_message>
<xml_diff>
--- a/Allegati/Requisiti.xlsx
+++ b/Allegati/Requisiti.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paolo\workspace\CPTRoverControl\Allegati\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17388214-567B-4F3D-B1F1-98A899501364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3254691E-7FE1-4B32-A63F-40DE357B4F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
   <si>
     <t>Descrizione del requisito</t>
   </si>
@@ -290,9 +290,6 @@
     <t>6 dipende da 4</t>
   </si>
   <si>
-    <t>9 sostituisce 3</t>
-  </si>
-  <si>
     <t>concordato</t>
   </si>
   <si>
@@ -316,6 +313,12 @@
 2 - molto importante
 3 - importante
 4 - secondario</t>
+  </si>
+  <si>
+    <t>L'app deve inviare tramite Bluetooth dei caratteri ASCII con una specifica formattazione</t>
+  </si>
+  <si>
+    <t>10 sostituisce 3</t>
   </si>
 </sst>
 </file>
@@ -1332,7 +1335,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:256" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
@@ -1381,7 +1384,7 @@
   <dimension ref="A1:BA39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1593,7 +1596,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="58" t="s">
         <v>23</v>
@@ -1609,7 +1612,7 @@
       </c>
       <c r="G4" s="40"/>
       <c r="H4" s="40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I4" s="19"/>
       <c r="J4" s="19"/>
@@ -1662,7 +1665,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>24</v>
@@ -1677,7 +1680,7 @@
         <v>4</v>
       </c>
       <c r="H5" s="40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I5" s="19"/>
       <c r="J5" s="19"/>
@@ -1730,7 +1733,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="59" t="s">
         <v>26</v>
@@ -1801,7 +1804,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="60" t="s">
         <v>25</v>
@@ -1817,7 +1820,7 @@
       </c>
       <c r="G7" s="41"/>
       <c r="H7" s="40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
@@ -1870,7 +1873,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="59" t="s">
         <v>21</v>
@@ -1888,7 +1891,7 @@
         <v>30</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I8" s="19"/>
       <c r="J8" s="19"/>
@@ -1941,7 +1944,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="60" t="s">
         <v>22</v>
@@ -1959,7 +1962,7 @@
         <v>31</v>
       </c>
       <c r="H9" s="40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I9" s="19"/>
       <c r="J9" s="19"/>
@@ -2012,10 +2015,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="51">
         <v>44806</v>
@@ -2027,7 +2030,7 @@
         <v>3</v>
       </c>
       <c r="H10" s="40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
@@ -2080,10 +2083,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="51">
         <v>44806</v>
@@ -2096,7 +2099,7 @@
       </c>
       <c r="G11" s="41"/>
       <c r="H11" s="40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I11" s="19"/>
       <c r="J11" s="19"/>
@@ -2144,18 +2147,18 @@
       <c r="AZ11" s="19"/>
       <c r="BA11" s="28"/>
     </row>
-    <row r="12" spans="1:53" s="16" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:53" s="16" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A12" s="30">
         <v>9</v>
       </c>
       <c r="B12" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="16" t="s">
-        <v>28</v>
+      <c r="C12" s="59" t="s">
+        <v>39</v>
       </c>
       <c r="D12" s="51">
-        <v>44813</v>
+        <v>44806</v>
       </c>
       <c r="E12" s="47">
         <v>1</v>
@@ -2163,11 +2166,9 @@
       <c r="F12" s="47">
         <v>1</v>
       </c>
-      <c r="G12" s="41" t="s">
+      <c r="G12" s="41"/>
+      <c r="H12" s="40" t="s">
         <v>32</v>
-      </c>
-      <c r="H12" s="40" t="s">
-        <v>33</v>
       </c>
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
@@ -2219,13 +2220,27 @@
       <c r="A13" s="30">
         <v>10</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="40"/>
+      <c r="B13" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="51">
+        <v>44813</v>
+      </c>
+      <c r="E13" s="47">
+        <v>1</v>
+      </c>
+      <c r="F13" s="47">
+        <v>1</v>
+      </c>
+      <c r="G13" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="40" t="s">
+        <v>32</v>
+      </c>
       <c r="I13" s="19"/>
       <c r="J13" s="19"/>
       <c r="K13" s="19"/>
@@ -2276,12 +2291,6 @@
       <c r="A14" s="30">
         <v>11</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="40"/>
       <c r="I14" s="19"/>
       <c r="J14" s="19"/>
       <c r="K14" s="19"/>
@@ -3350,8 +3359,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F65536">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="F15:F65536 F2:F13">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3362,8 +3371,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4:E34">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="E15:E34 E4:E13">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>